<commit_message>
Ok I pull up
</commit_message>
<xml_diff>
--- a/Comportamento_Normal.xlsx
+++ b/Comportamento_Normal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossie\Desktop\Projeto Aplicado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C80105C9-5F25-4A9C-A55E-DA49E5B612D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC2CFBF-9006-46CE-88CF-ECB48A563DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AFD8EB35-9D61-49A0-9C84-3E618A8CD7AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AFD8EB35-9D61-49A0-9C84-3E618A8CD7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -360,6 +360,45 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -369,46 +408,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -725,176 +725,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B56130-EA4D-4471-893A-01BED45CDDFE}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="2:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="2:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="16" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="16" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="16" t="s">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="16" t="s">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="16" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="16" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="6"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="A6:C12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:D14"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>